<commit_message>
updated foxBMS-slave to version 2.02
</commit_message>
<xml_diff>
--- a/BMS-Interface/foxBMS_BMS-Interface_BOM.xlsx
+++ b/BMS-Interface/foxBMS_BMS-Interface_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="5400" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="360" yWindow="360" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="foxBMS_BMS-Interface" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
   <si>
     <t>Qty</t>
   </si>
@@ -58,6 +58,9 @@
     <t>C301, C302, C401, C402</t>
   </si>
   <si>
+    <t>0R</t>
+  </si>
+  <si>
     <t>1.21k</t>
   </si>
   <si>
@@ -67,12 +70,6 @@
     <t>R501, R502</t>
   </si>
   <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>C501, C503</t>
-  </si>
-  <si>
     <t>27pF</t>
   </si>
   <si>
@@ -88,12 +85,12 @@
     <t>R311, R411</t>
   </si>
   <si>
-    <t>HX1188NL</t>
-  </si>
-  <si>
     <t>T501, T502</t>
   </si>
   <si>
+    <t>LTC6820</t>
+  </si>
+  <si>
     <t>MSOP16</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
     <t>Mouser</t>
   </si>
   <si>
-    <t>553-1340-ND</t>
-  </si>
-  <si>
     <t>LTC6820HMS#PBF-ND</t>
   </si>
   <si>
@@ -148,19 +142,19 @@
     <t>R301, R303, R306, R309, R401, R403, R406, R409</t>
   </si>
   <si>
+    <t>HM2102NL</t>
+  </si>
+  <si>
+    <t>C_0603</t>
+  </si>
+  <si>
+    <t>R_0603</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
     <t>Resistor</t>
-  </si>
-  <si>
-    <t>Capacitor</t>
-  </si>
-  <si>
-    <t>R_0603</t>
-  </si>
-  <si>
-    <t>C_0603</t>
-  </si>
-  <si>
-    <t>LTC6820HMS#PBF</t>
   </si>
 </sst>
 </file>
@@ -1015,10 +1009,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1029,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1056,18 +1050,18 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -1091,17 +1085,17 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -1115,17 +1109,17 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -1139,16 +1133,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="3">
+        <v>39</v>
+      </c>
+      <c r="B5" s="4">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E5" s="3">
         <v>603</v>
@@ -1165,25 +1159,25 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="3">
+        <v>39</v>
+      </c>
+      <c r="B6" s="4">
         <v>8</v>
       </c>
-      <c r="C6" s="3">
-        <v>0</v>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E6" s="3">
         <v>603</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H6" s="3">
         <v>2059527</v>
@@ -1191,25 +1185,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="3">
+        <v>39</v>
+      </c>
+      <c r="B7" s="4">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" s="3">
         <v>603</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H7" s="3">
         <v>2059331</v>
@@ -1217,25 +1211,25 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="3">
+        <v>39</v>
+      </c>
+      <c r="B8" s="4">
         <v>2</v>
       </c>
       <c r="C8" s="3">
         <v>120</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E8" s="3">
         <v>603</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H8" s="3">
         <v>2303067</v>
@@ -1243,68 +1237,68 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="3">
+        <v>39</v>
+      </c>
+      <c r="B9" s="4">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3">
         <v>603</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
         <v>45</v>
       </c>
       <c r="H9" s="3">
-        <v>1907343</v>
+        <v>1414627</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2</v>
+        <v>39</v>
+      </c>
+      <c r="B10" s="4">
+        <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E10" s="3">
         <v>603</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H10" s="3">
-        <v>1414627</v>
+        <v>2059343</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="3">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>39</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>806</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E11" s="3">
         <v>603</v>
@@ -1313,43 +1307,37 @@
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H11" s="3">
-        <v>2059343</v>
+        <v>2059324</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="3">
+        <v>39</v>
+      </c>
+      <c r="B12" s="4">
         <v>2</v>
       </c>
-      <c r="C12" s="3">
-        <v>806</v>
+      <c r="C12" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="3">
-        <v>603</v>
+        <v>42</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="F12" t="s">
         <v>23</v>
-      </c>
-      <c r="G12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="3">
-        <v>2059324</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="3">
+        <v>39</v>
+      </c>
+      <c r="B13" s="4">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1359,61 +1347,38 @@
         <v>24</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="3">
+        <v>603</v>
+      </c>
+      <c r="F14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="3">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="3">
-        <v>8</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="G14" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="3">
-        <v>603</v>
-      </c>
-      <c r="F15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" s="3">
+      <c r="H14" s="3">
         <v>2059527</v>
       </c>
     </row>

</xml_diff>